<commit_message>
Atualizar dados de consulta
</commit_message>
<xml_diff>
--- a/retomada_presencial/Retomada Presencial das Aulas.xlsx
+++ b/retomada_presencial/Retomada Presencial das Aulas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="335">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="341">
   <x:si>
     <x:t xml:space="preserve">ID</x:t>
   </x:si>
@@ -1030,6 +1030,24 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Fabíola Gonçalves</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">jean.ferreira10@fatec.sp.gov.br</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">JEAN FERREIRA</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">jean carlo ferreira</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">ricardo.oliveira71@fatec.sp.gov.br</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">RICARDO OLIVEIRA</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Ricardo Magalhães de Oliveira</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1126,8 +1144,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AE105" insertRow="1" totalsRowShown="0">
-  <x:autoFilter ref="A1:AE105"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AE107" insertRow="1" totalsRowShown="0">
+  <x:autoFilter ref="A1:AE107"/>
   <x:tableColumns count="31">
     <x:tableColumn id="1" uniqueName="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" uniqueName="2" name="Hora de início" dataDxfId="3"/>
@@ -7608,11 +7626,127 @@
       <x:c r="AD105"/>
       <x:c r="AE105" s="10" t="s"/>
     </x:row>
+    <x:row r="106" hidden="0">
+      <x:c r="A106">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B106" s="2">
+        <x:v>44468.4700115741</x:v>
+      </x:c>
+      <x:c r="C106" s="2">
+        <x:v>44468.4708333333</x:v>
+      </x:c>
+      <x:c r="D106" s="10" t="s">
+        <x:v>335</x:v>
+      </x:c>
+      <x:c r="E106" s="10" t="s">
+        <x:v>336</x:v>
+      </x:c>
+      <x:c r="F106"/>
+      <x:c r="G106" s="10" t="s"/>
+      <x:c r="H106" s="10" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="I106"/>
+      <x:c r="J106" s="10" t="s"/>
+      <x:c r="K106" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="L106"/>
+      <x:c r="M106" s="10" t="s"/>
+      <x:c r="N106" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="O106"/>
+      <x:c r="P106" s="10" t="s"/>
+      <x:c r="Q106" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="R106"/>
+      <x:c r="S106" s="10" t="s"/>
+      <x:c r="T106" s="10" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="U106"/>
+      <x:c r="V106" s="10" t="s"/>
+      <x:c r="W106" s="10" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="X106"/>
+      <x:c r="Y106" s="10" t="s"/>
+      <x:c r="Z106" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="AA106"/>
+      <x:c r="AB106" s="10" t="s"/>
+      <x:c r="AC106" s="10" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="AD106"/>
+      <x:c r="AE106" s="10" t="s"/>
+    </x:row>
+    <x:row r="107" hidden="0">
+      <x:c r="A107">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="B107" s="2">
+        <x:v>44468.7959027778</x:v>
+      </x:c>
+      <x:c r="C107" s="2">
+        <x:v>44468.796412037</x:v>
+      </x:c>
+      <x:c r="D107" s="10" t="s">
+        <x:v>338</x:v>
+      </x:c>
+      <x:c r="E107" s="10" t="s">
+        <x:v>339</x:v>
+      </x:c>
+      <x:c r="F107"/>
+      <x:c r="G107" s="10" t="s"/>
+      <x:c r="H107" s="10" t="s">
+        <x:v>340</x:v>
+      </x:c>
+      <x:c r="I107"/>
+      <x:c r="J107" s="10" t="s"/>
+      <x:c r="K107" s="10" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="L107"/>
+      <x:c r="M107" s="10" t="s"/>
+      <x:c r="N107" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="O107"/>
+      <x:c r="P107" s="10" t="s"/>
+      <x:c r="Q107" s="10" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="R107"/>
+      <x:c r="S107" s="10" t="s"/>
+      <x:c r="T107" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="U107"/>
+      <x:c r="V107" s="10" t="s"/>
+      <x:c r="W107" s="10" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="X107"/>
+      <x:c r="Y107" s="10" t="s"/>
+      <x:c r="Z107" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AA107"/>
+      <x:c r="AB107" s="10" t="s"/>
+      <x:c r="AC107" s="10" t="s"/>
+      <x:c r="AD107"/>
+      <x:c r="AE107" s="10" t="s"/>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <x:tableParts count="1">
-    <x:tablePart r:id="R49bd0e5b3574472e"/>
+    <x:tablePart r:id="Rae0a845600fa4f4f"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>